<commit_message>
[Shubham] Updated at 9-9-24
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking117.xlsx
+++ b/data/excel/FlightBooking117.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89828186-1C09-464E-A419-D0A050AFDDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0501C4FF-DAE0-494E-97B3-6EF81DD74398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="13" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -33,7 +33,9 @@
     <sheet name="Sheet11" sheetId="97" r:id="rId18"/>
     <sheet name="NonBranding" sheetId="96" r:id="rId19"/>
     <sheet name="Liveupdate117" sheetId="98" r:id="rId20"/>
-    <sheet name="Sheet17" sheetId="95" r:id="rId21"/>
+    <sheet name="Sheet15" sheetId="99" r:id="rId21"/>
+    <sheet name="Sheet16" sheetId="100" r:id="rId22"/>
+    <sheet name="Sheet17" sheetId="95" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9738" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10559" uniqueCount="542">
   <si>
     <t>del</t>
   </si>
@@ -23264,8 +23266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770F2E9B-7EB4-4DA2-A71C-401253060AA1}">
   <dimension ref="A1:BW15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26896,11 +26898,3371 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F3D401-7E84-4C94-B186-4611925D2206}">
+  <dimension ref="A1:BW11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BJ1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BO1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB2" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC2" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS2" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB3" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC3" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL3" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP3" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS3" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ4" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR4" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA4" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB4" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC4" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD4" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF4" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL4" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP4" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS4" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW4" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Z5" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB5" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC5" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD5" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF5" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL5" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP5" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS5" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT5" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW5" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z6" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK6" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS6" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT6" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU6" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ6" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA6" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB6" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC6" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD6" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF6" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH6" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK6" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL6" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM6" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP6" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS6" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT6" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW6" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R7" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z7" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK7" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO7" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP7" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ7" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR7" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS7" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT7" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU7" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ7" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA7" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB7" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC7" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD7" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE7" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF7" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH7" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK7" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL7" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM7" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP7" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS7" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT7" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW7" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R8" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X8" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z8" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA8" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB8" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE8" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK8" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO8" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP8" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ8" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="AR8" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="AS8" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AT8" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AU8" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ8" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA8" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB8" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC8" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD8" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE8" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF8" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH8" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK8" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL8" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM8" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP8" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS8" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT8" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU8" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW8" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R9" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z9" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA9" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB9" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO9" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP9" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ9" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="AR9" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="AS9" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AT9" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AU9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ9" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA9" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB9" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC9" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD9" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF9" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH9" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI9" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK9" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL9" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM9" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP9" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS9" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT9" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU9" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW9" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R10" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W10" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z10" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA10" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AB10" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK10" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO10" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP10" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ10" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="AR10" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="AS10" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT10" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU10" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ10" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA10" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB10" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC10" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD10" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE10" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF10" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK10" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL10" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM10" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP10" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS10" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT10" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU10" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW10" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R11" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Z11" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA11" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="AB11" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK11" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO11" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ11" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="AR11" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="AS11" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT11" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU11" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ11" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA11" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB11" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC11" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD11" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE11" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF11" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH11" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK11" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL11" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM11" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP11" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS11" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT11" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW11" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R11" xr:uid="{E7C2F757-E578-4A50-B438-C3416B49AC84}">
+      <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU11" xr:uid="{8E1870E0-E674-4FB1-8E9C-AD21E364859A}">
+      <formula1>"LCC,LCC+GDS,GDS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G11" xr:uid="{80BB3EF1-B090-4849-8CF7-418FE4BA5806}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H11" xr:uid="{2BD8D39F-C115-4ABF-BBD6-3B0CF45B1230}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11" xr:uid="{4D77A095-A730-4B01-AA52-ACF01A55D481}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11 BW2:BW11" xr:uid="{E999A00F-0D7B-4796-B29A-99B9857F5468}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z11" xr:uid="{BD355A7A-2D3A-403D-A2EA-9FEDF015AD9E}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR11" xr:uid="{1620670C-E004-43BB-AEE8-7078737981D2}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P11" xr:uid="{02C56D05-A6DD-41B1-9E8C-B5F6067C754D}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2:BS11 AP2:AP11 AK2:AK11 AN2:AN11" xr:uid="{F5D86A24-A598-4855-A86D-2ADBB4787114}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2:BR11" xr:uid="{CC99464C-2F0D-48AF-97B4-7EAC198D6732}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM11" xr:uid="{FC75C488-BAA8-446D-9EAC-57C198FA7416}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{426DAA89-FF6B-4799-8DBC-4BDB7D2E8D3A}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{8D5B663A-93F9-432B-A201-CA5C25F5495C}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11 BO2:BO11 AC2:AC11" xr:uid="{CE820163-5FB8-4FA2-8C87-26015027B8A0}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O11" xr:uid="{EAF210FF-AD36-49DB-A5A0-2ADF1E9DE8F6}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH11" xr:uid="{76043091-7B8D-4399-AB58-B1CEB4510230}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM11" xr:uid="{E96D71B7-37E0-46AD-9EC0-5E8435C29999}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK11" xr:uid="{754FA178-0457-4E70-BEC0-CF5458B6D456}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S11" xr:uid="{2BDF30F5-A2CE-4FB9-B451-F91694056E66}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T11" xr:uid="{84CCC2CA-8B81-4558-925B-4FA00F0FDF8C}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U11" xr:uid="{B8D9F2DD-8813-4043-94D6-66B1A8B372DE}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY11" xr:uid="{AD9D0CC7-712A-4019-99B9-4ACFB896913B}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11 AD2:AD11" xr:uid="{BE182EC9-4793-4ECA-B052-E768F4F4C3C4}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL11" xr:uid="{65F4CE59-2A55-481E-BEE4-675FCF2BC486}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q11" xr:uid="{040B671D-D3B4-4118-9C55-560AC9DA6BD7}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH11" xr:uid="{77177A79-0D45-4D24-AC58-E92F7B0AD765}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI11" xr:uid="{5800AE6E-8F13-4128-8F77-154828B7C6D7}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11" xr:uid="{C4F90AFE-A9EE-4A68-84BF-7DCA343463BE}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT11" xr:uid="{3B30E2AD-F0EE-41C6-8132-921243139E78}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO11" xr:uid="{F989D5B8-61F2-4F48-8BE7-85613FCC8687}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11" xr:uid="{D2CDE9EF-7F4A-46FC-AC85-621EEB792FF7}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{511F3680-FAD9-4F2F-A1A6-46DF72847E27}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{0362FD13-DFFD-470C-A3EC-47692F24DB15}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{B1CD087C-3220-45D7-A1DA-1AC2CAB21FAB}"/>
+    <hyperlink ref="I3:I9" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{F35FCC5A-85A0-407E-9F11-34C5BDD97ECA}"/>
+    <hyperlink ref="R3:R9" r:id="rId5" display="ajit.kumar@quadlabs.com" xr:uid="{DECA4B0C-9D07-4989-A494-E34AD559723A}"/>
+    <hyperlink ref="I7" r:id="rId6" display="shekhar.singh@quadlabs.com" xr:uid="{35EF142D-FFCC-4F2C-AF73-83DDDABF697F}"/>
+    <hyperlink ref="R7" r:id="rId7" display="ajit.kumar@quadlabs.com" xr:uid="{165030BD-4C96-4979-8DD6-E793153BF030}"/>
+    <hyperlink ref="I4" r:id="rId8" display="shekhar.singh@quadlabs.com" xr:uid="{493A319C-9F11-4054-9766-E67060909026}"/>
+    <hyperlink ref="R4" r:id="rId9" display="ajit.kumar@quadlabs.com" xr:uid="{9C130085-47E2-478B-A11F-C801949D11E4}"/>
+    <hyperlink ref="I8" r:id="rId10" display="shekhar.singh@quadlabs.com" xr:uid="{1545DBF1-C67C-4B32-BE93-361B608383E8}"/>
+    <hyperlink ref="R8" r:id="rId11" display="ajit.kumar@quadlabs.com" xr:uid="{C54AA73E-BF65-4665-93BC-FC6BDC18A00C}"/>
+    <hyperlink ref="N3" r:id="rId12" display="Admin@123" xr:uid="{7FD23657-DEA2-4ECE-B3F7-CAEEE97B538B}"/>
+    <hyperlink ref="N4" r:id="rId13" display="Admin@123" xr:uid="{E82BB802-55BB-4990-98D9-9AC8D47F5A3E}"/>
+    <hyperlink ref="N5" r:id="rId14" display="Admin@123" xr:uid="{D6C1D293-3342-42DF-8AE2-F1EC4330D844}"/>
+    <hyperlink ref="N6" r:id="rId15" display="Admin@123" xr:uid="{E0EEC9F2-9F3C-4F3E-A172-1B05B150397F}"/>
+    <hyperlink ref="N7" r:id="rId16" display="Admin@123" xr:uid="{DE7E6999-2B58-4B89-8136-D5494DE44678}"/>
+    <hyperlink ref="N8" r:id="rId17" display="Admin@123" xr:uid="{79447081-020E-4CBA-A2E2-AA6779A369A2}"/>
+    <hyperlink ref="N9" r:id="rId18" display="Admin@123" xr:uid="{E4A31E91-7EB8-48F1-B1DB-77D19EC1BBAF}"/>
+    <hyperlink ref="N10" r:id="rId19" display="Admin@123" xr:uid="{007E928C-A05A-43B9-AE4E-E7C85789F3A3}"/>
+    <hyperlink ref="I10" r:id="rId20" display="shekhar.singh@quadlabs.com" xr:uid="{751B98D6-3036-46C6-890D-F37B2E4AB6A6}"/>
+    <hyperlink ref="R10" r:id="rId21" display="ajit.kumar@quadlabs.com" xr:uid="{B1660E69-EFC2-4FA9-A2A9-7E6A7BFA500C}"/>
+    <hyperlink ref="I11" r:id="rId22" display="shekhar.singh@quadlabs.com" xr:uid="{B9FA0E7D-B59E-4CE6-B840-FEE85B394648}"/>
+    <hyperlink ref="R11" r:id="rId23" display="ajit.kumar@quadlabs.com" xr:uid="{18BE8DAE-1064-46F5-95F6-85CA79235B10}"/>
+    <hyperlink ref="N11" r:id="rId24" display="Admin@123" xr:uid="{708FB43E-0C0C-4286-97C4-8A1005A7D00B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D52D2FB-7FAD-4F3F-9A09-4A7C32570156}">
+  <dimension ref="A1:BW2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BK7" sqref="BK7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BJ1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BO1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB2" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC2" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS2" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{E37BD82A-B953-473D-A7D9-73F38D4D1AA2}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{A0BA1EEF-B70A-47E2-9C9E-936A86D38C0E}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{D5AE3FCC-85B6-476B-9B83-634841FE5AF4}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{B44B8568-30D8-4B79-B9A8-884CEA2789A5}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2" xr:uid="{A7ECB280-A86F-48BA-951C-CC6AF7BBFEC3}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{70F14FE4-10ED-42E3-AFB1-DB1166C00608}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{50D69318-4B1F-464D-B7A9-AFD5A1D6CE2F}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{9077C7E9-97F2-4BB0-98B2-006E2ED17B05}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 AD2" xr:uid="{ADB078B1-6207-4E23-B3C0-65E919EE9A01}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{5471B428-99F0-4523-85E6-1740DDF054CB}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{A4A7A7E4-8BC2-4081-A3F1-8BE6895FE004}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{226551C0-716C-4143-B4D0-DD3EF5E2B0A8}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{1C53A769-76A4-42B7-9FE1-223054B7FCD2}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{ECEC641B-EC4D-4F09-8020-C50104CF3925}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{B4CB4233-AAC0-4608-915F-37E4A06721A9}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH2" xr:uid="{EE66DE2A-7DE5-494A-BF5D-E57F31DFD14C}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{3F137DC0-C1E7-43B8-97C6-3E52D264314E}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 BO2 AC2" xr:uid="{6504A1FE-63DC-48D5-AEA1-4B61A033C77A}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{C24A934C-1C56-4D9B-9564-019F1EA3329C}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{B41949E4-B938-4FAB-8BAB-9AAB329A4408}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2" xr:uid="{673B7394-FA3A-4A50-AFF1-BEBF8F02D671}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2" xr:uid="{A8242708-E6D0-492D-BC26-C62DA16FE317}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2 AP2 AK2 AN2" xr:uid="{1B03B5B4-BBC8-4FD2-9215-7CAC67B3BAA6}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{F1130A5A-3830-496A-9D7C-FA29CA330C2A}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{C702DD6E-C27C-41A5-A136-B5741C020696}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{D0ADBC6A-9875-46F1-8B5B-4D175FD6B1F7}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 BW2" xr:uid="{28F5EFF9-615E-41B4-B47D-ACDA3ADDC827}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{345E694D-72BD-46BF-90A6-09478E3757A3}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{C99BA959-8BED-49D9-AE9E-478A84F3A217}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{3D74487B-0840-4A41-8CC6-52DC10635AF9}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{E2B50CDA-A4F2-45B1-8253-7FB33596CD4D}">
+      <formula1>"LCC,LCC+GDS,GDS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{65DE4F97-C6CA-41F5-88FA-3737969E0509}">
+      <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{9132859E-0270-4FAA-B752-BE0E692CF41F}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{018C4B47-CA9C-4B0F-832F-898E38B925F2}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{B522FF91-D972-4094-847E-337E32F67679}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4DC434-9680-44B9-B67E-2B0017A95C76}">
   <dimension ref="A1:BW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>